<commit_message>
Edição para classes e ids
</commit_message>
<xml_diff>
--- a/cores.xlsx
+++ b/cores.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PraticaDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2096604-14DB-44C2-BB62-508A27622AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB98FAD8-D036-41F9-8E1E-FA8F2A31C784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="cores" sheetId="1" r:id="rId1"/>
+    <sheet name="classe e id" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Hexadecimal</t>
   </si>
@@ -77,6 +78,27 @@
   </si>
   <si>
     <t>#C74A4C</t>
+  </si>
+  <si>
+    <t>Tendo em observação que o conteudo dessa planilha esta faltando devido á ter sido iniciada bem depois</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>Função</t>
+  </si>
+  <si>
+    <t>obs</t>
   </si>
 </sst>
 </file>
@@ -265,7 +287,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +320,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -584,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +636,7 @@
     <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="108" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,6 +685,9 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -789,4 +836,295 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F9457D-2E4E-45CB-AD1B-0A01934B8197}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="17" customWidth="1"/>
+    <col min="3" max="4" width="9.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>